<commit_message>
Updated TC numbers and status
</commit_message>
<xml_diff>
--- a/S1000/S1000 Test Parameters.xlsx
+++ b/S1000/S1000 Test Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nventco-my.sharepoint.com/personal/e1176752_nventco_com/Documents/Documents/VSCode/Projects/LPSD/LPSD/S1000/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04934AEF-6842-4F89-A37A-AF54107AE78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{04934AEF-6842-4F89-A37A-AF54107AE78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9B27004-57C7-43C5-A2D1-D179DF2A63E0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="26">
   <si>
     <t>Test Results S1000</t>
   </si>
@@ -81,6 +81,39 @@
   </si>
   <si>
     <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Ready for testing</t>
+  </si>
+  <si>
+    <t>Graitec/ASTI</t>
+  </si>
+  <si>
+    <t>Needs review</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>Needs SI45i change</t>
+  </si>
+  <si>
+    <t>Created as TC17</t>
+  </si>
+  <si>
+    <t>Created as TC18</t>
+  </si>
+  <si>
+    <t>Created as TC19</t>
   </si>
 </sst>
 </file>
@@ -158,7 +191,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -181,25 +214,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -216,11 +246,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,49 +540,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="6" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:9" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="8" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B8" s="5" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="8" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="11" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="2"/>
+      <c r="G8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -555,14 +602,21 @@
       <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="13"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="5"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -572,16 +626,25 @@
       <c r="D11" s="2">
         <v>42.43</v>
       </c>
-      <c r="E11" s="10" t="str">
+      <c r="E11" s="5" t="str">
         <f t="shared" ref="E11:E29" si="0">"S1000 QA TC"&amp;F11</f>
         <v>S1000 QA TC16</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <f t="shared" ref="F11:F12" si="1">F12+1</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
@@ -591,16 +654,22 @@
       <c r="D12" s="2">
         <v>48.99</v>
       </c>
-      <c r="E12" s="10" t="str">
+      <c r="E12" s="5" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC15</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
@@ -610,16 +679,22 @@
       <c r="D13" s="2">
         <v>57.45</v>
       </c>
-      <c r="E13" s="10" t="str">
+      <c r="E13" s="5" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC14</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <f>F14+1</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
@@ -629,21 +704,49 @@
       <c r="D14" s="2">
         <v>64.81</v>
       </c>
-      <c r="E14" s="10" t="str">
+      <c r="E14" s="5" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC13</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <f>F19+1</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B16" s="5" t="s">
+      <c r="G14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -655,11 +758,19 @@
       <c r="D17" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
@@ -671,13 +782,19 @@
       <c r="D19" s="2">
         <v>58.09</v>
       </c>
-      <c r="E19" s="10" t="str">
+      <c r="E19" s="5" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC12</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <f t="shared" ref="F19:F20" si="2">F20+1</f>
         <v>12</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -690,13 +807,22 @@
       <c r="D20" s="2">
         <v>65.38</v>
       </c>
-      <c r="E20" s="10" t="str">
+      <c r="E20" s="5" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC11</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <f t="shared" si="2"/>
         <v>11</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -709,13 +835,19 @@
       <c r="D21" s="2">
         <v>75</v>
       </c>
-      <c r="E21" s="10" t="str">
+      <c r="E21" s="5" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC10</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <f>F22+1</f>
         <v>10</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -728,21 +860,46 @@
       <c r="D22" s="2">
         <v>83.52</v>
       </c>
-      <c r="E22" s="10" t="str">
+      <c r="E22" s="5" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC9</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <f>F27+1</f>
         <v>9</v>
       </c>
+      <c r="G22" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
@@ -754,11 +911,19 @@
       <c r="D25" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
@@ -770,13 +935,19 @@
       <c r="D27" s="4">
         <v>42.43</v>
       </c>
-      <c r="E27" s="10" t="str">
+      <c r="E27" s="5" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC8</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <f t="shared" ref="F27:F28" si="3">F28+1</f>
         <v>8</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -789,13 +960,19 @@
       <c r="D28" s="4">
         <v>48.99</v>
       </c>
-      <c r="E28" s="10" t="str">
+      <c r="E28" s="5" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC7</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <f t="shared" si="3"/>
         <v>7</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -809,13 +986,19 @@
       <c r="D29" s="4">
         <v>57.45</v>
       </c>
-      <c r="E29" s="10" t="str">
+      <c r="E29" s="5" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC6</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <f>F30+1</f>
         <v>6</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -828,23 +1011,48 @@
       <c r="D30" s="4">
         <v>64.81</v>
       </c>
-      <c r="E30" s="10" t="str">
+      <c r="E30" s="5" t="str">
         <f>"S1000 QA TC"&amp;F30</f>
         <v>S1000 QA TC5</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <f>F35+1</f>
         <v>5</v>
       </c>
+      <c r="G30" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>3</v>
       </c>
@@ -854,13 +1062,21 @@
       <c r="D33" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="13"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="5"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>6</v>
       </c>
@@ -870,15 +1086,21 @@
       <c r="D35" s="2">
         <v>78.58</v>
       </c>
-      <c r="E35" s="10" t="str">
+      <c r="E35" s="5" t="str">
         <f t="shared" ref="E35:E37" si="4">"S1000 QA TC"&amp;F35</f>
         <v>S1000 QA TC4</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>7</v>
       </c>
@@ -888,15 +1110,21 @@
       <c r="D36" s="2">
         <v>86.46</v>
       </c>
-      <c r="E36" s="10" t="str">
+      <c r="E36" s="5" t="str">
         <f t="shared" si="4"/>
         <v>S1000 QA TC3</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>8</v>
       </c>
@@ -906,15 +1134,21 @@
       <c r="D37" s="2">
         <v>97.08</v>
       </c>
-      <c r="E37" s="10" t="str">
+      <c r="E37" s="5" t="str">
         <f t="shared" si="4"/>
         <v>S1000 QA TC2</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>9</v>
       </c>
@@ -924,28 +1158,66 @@
       <c r="D38" s="2">
         <v>106.65</v>
       </c>
-      <c r="E38" s="10" t="str">
+      <c r="E38" s="5" t="str">
         <f>"S1000 QA TC"&amp;F38</f>
         <v>S1000 QA TC1</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>1</v>
       </c>
+      <c r="G38" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="17">
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E24:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Notes xmlns="874d5487-6c76-4636-9554-18c8210b1644" xsi:nil="true"/>
+    <TaxCatchAll xmlns="053b13a0-8fcf-4745-a4a1-7bc77e471615" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="874d5487-6c76-4636-9554-18c8210b1644">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CE6C5D91432E0C44B4C6A820EB7148C0" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7bf22301abfb8b95bc051eca2bbc6e31">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="874d5487-6c76-4636-9554-18c8210b1644" xmlns:ns3="053b13a0-8fcf-4745-a4a1-7bc77e471615" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b6d9a428d9d7edc7a0a919696afeea0" ns2:_="" ns3:_="">
     <xsd:import namespace="874d5487-6c76-4636-9554-18c8210b1644"/>
@@ -1188,28 +1460,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Notes xmlns="874d5487-6c76-4636-9554-18c8210b1644" xsi:nil="true"/>
-    <TaxCatchAll xmlns="053b13a0-8fcf-4745-a4a1-7bc77e471615" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="874d5487-6c76-4636-9554-18c8210b1644">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4DDB590-B31D-4E3A-91E0-F94966B82335}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACAC892F-15D7-4937-AF88-9DDDD5A9DFE5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="874d5487-6c76-4636-9554-18c8210b1644"/>
+    <ds:schemaRef ds:uri="053b13a0-8fcf-4745-a4a1-7bc77e471615"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A22604BF-35E4-4972-8131-FFAD3720D651}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1226,23 +1496,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACAC892F-15D7-4937-AF88-9DDDD5A9DFE5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="874d5487-6c76-4636-9554-18c8210b1644"/>
-    <ds:schemaRef ds:uri="053b13a0-8fcf-4745-a4a1-7bc77e471615"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4DDB590-B31D-4E3A-91E0-F94966B82335}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ran test on June 4, proof of concept for getting protectedpoint
</commit_message>
<xml_diff>
--- a/S1000/S1000 Test Parameters.xlsx
+++ b/S1000/S1000 Test Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nventco-my.sharepoint.com/personal/e1176752_nventco_com/Documents/Documents/VSCode/Projects/LPSD/LPSD/S1000/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nventco-my.sharepoint.com/personal/e2023355_nventco_com/Documents/Documents/VSCode/Projects/LPSD/S1000/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="73" documentId="8_{04934AEF-6842-4F89-A37A-AF54107AE78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9B27004-57C7-43C5-A2D1-D179DF2A63E0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="6852" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -230,6 +230,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -242,22 +258,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,10 +538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +551,7 @@
     <col min="3" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="6" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
@@ -569,26 +570,26 @@
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
     </row>
     <row r="8" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="13" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -602,10 +603,10 @@
       <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="13"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -613,7 +614,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="5"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="14"/>
+      <c r="G10" s="8"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -634,7 +635,7 @@
         <f t="shared" ref="F11:F12" si="1">F12+1</f>
         <v>16</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="9" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="4" t="s">
@@ -662,7 +663,7 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -687,7 +688,7 @@
         <f>F14+1</f>
         <v>14</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -712,7 +713,7 @@
         <f>F19+1</f>
         <v>13</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="9" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="4" t="s">
@@ -728,23 +729,23 @@
       <c r="D15" s="2"/>
       <c r="E15" s="5"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="14"/>
+      <c r="G15" s="8"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="13" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -758,10 +759,10 @@
       <c r="D17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="13"/>
+      <c r="E17" s="11"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
@@ -769,7 +770,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="14"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -790,7 +791,7 @@
         <f t="shared" ref="F19:F20" si="2">F20+1</f>
         <v>12</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -815,13 +816,13 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="9" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -843,7 +844,7 @@
         <f>F22+1</f>
         <v>10</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -868,7 +869,7 @@
         <f>F27+1</f>
         <v>9</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H22" s="2" t="s">
@@ -881,23 +882,23 @@
       <c r="D23" s="2"/>
       <c r="E23" s="5"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="14"/>
+      <c r="G23" s="8"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="13" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F24" s="2"/>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -911,10 +912,10 @@
       <c r="D25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="13"/>
+      <c r="E25" s="11"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
@@ -922,7 +923,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="14"/>
+      <c r="G26" s="8"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
@@ -943,7 +944,7 @@
         <f t="shared" ref="F27:F28" si="3">F28+1</f>
         <v>8</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H27" s="2" t="s">
@@ -968,7 +969,7 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H28" s="2" t="s">
@@ -994,7 +995,7 @@
         <f>F30+1</f>
         <v>6</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H29" s="2" t="s">
@@ -1019,7 +1020,7 @@
         <f>F35+1</f>
         <v>5</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H30" s="2" t="s">
@@ -1032,23 +1033,23 @@
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="14"/>
+      <c r="G31" s="8"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="13" t="s">
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="2"/>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H32" s="13" t="s">
+      <c r="H32" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1062,10 +1063,10 @@
       <c r="D33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="13"/>
+      <c r="E33" s="11"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
@@ -1073,7 +1074,7 @@
       <c r="D34" s="2"/>
       <c r="E34" s="5"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="14"/>
+      <c r="G34" s="8"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -1093,7 +1094,7 @@
       <c r="F35" s="2">
         <v>4</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H35" s="2" t="s">
@@ -1117,7 +1118,7 @@
       <c r="F36" s="2">
         <v>3</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H36" s="2" t="s">
@@ -1141,7 +1142,7 @@
       <c r="F37" s="2">
         <v>2</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="G37" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H37" s="2" t="s">
@@ -1165,7 +1166,7 @@
       <c r="F38" s="2">
         <v>1</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H38" s="2" t="s">
@@ -1174,11 +1175,9 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E24:E25"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
@@ -1188,36 +1187,18 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Notes xmlns="874d5487-6c76-4636-9554-18c8210b1644" xsi:nil="true"/>
-    <TaxCatchAll xmlns="053b13a0-8fcf-4745-a4a1-7bc77e471615" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="874d5487-6c76-4636-9554-18c8210b1644">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CE6C5D91432E0C44B4C6A820EB7148C0" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7bf22301abfb8b95bc051eca2bbc6e31">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="874d5487-6c76-4636-9554-18c8210b1644" xmlns:ns3="053b13a0-8fcf-4745-a4a1-7bc77e471615" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b6d9a428d9d7edc7a0a919696afeea0" ns2:_="" ns3:_="">
     <xsd:import namespace="874d5487-6c76-4636-9554-18c8210b1644"/>
@@ -1460,10 +1441,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Notes xmlns="874d5487-6c76-4636-9554-18c8210b1644" xsi:nil="true"/>
+    <TaxCatchAll xmlns="053b13a0-8fcf-4745-a4a1-7bc77e471615" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="874d5487-6c76-4636-9554-18c8210b1644">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4DDB590-B31D-4E3A-91E0-F94966B82335}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A22604BF-35E4-4972-8131-FFAD3720D651}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="874d5487-6c76-4636-9554-18c8210b1644"/>
+    <ds:schemaRef ds:uri="053b13a0-8fcf-4745-a4a1-7bc77e471615"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1480,20 +1493,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A22604BF-35E4-4972-8131-FFAD3720D651}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4DDB590-B31D-4E3A-91E0-F94966B82335}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="874d5487-6c76-4636-9554-18c8210b1644"/>
-    <ds:schemaRef ds:uri="053b13a0-8fcf-4745-a4a1-7bc77e471615"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated changes from Graitec push
</commit_message>
<xml_diff>
--- a/S1000/S1000 Test Parameters.xlsx
+++ b/S1000/S1000 Test Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nventco-my.sharepoint.com/personal/e2023355_nventco_com/Documents/Documents/VSCode/Projects/LPSD/S1000/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nventco-my.sharepoint.com/personal/e1176752_nventco_com/Documents/Documents/VSCode/Projects/LPSD/LPSD/S1000/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{04934AEF-6842-4F89-A37A-AF54107AE78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9B27004-57C7-43C5-A2D1-D179DF2A63E0}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="8_{04934AEF-6842-4F89-A37A-AF54107AE78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D4DAE17-D051-495F-AC87-EDF3E96A5668}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="6852" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="22">
   <si>
     <t>Test Results S1000</t>
   </si>
@@ -71,9 +71,6 @@
     <t>SI40i</t>
   </si>
   <si>
-    <t xml:space="preserve">SI45i, WRONG CALCULATIONS, BELONG TO SI25i  </t>
-  </si>
-  <si>
     <t>SI60i</t>
   </si>
   <si>
@@ -86,12 +83,6 @@
     <t>Ready for testing</t>
   </si>
   <si>
-    <t>Graitec/ASTI</t>
-  </si>
-  <si>
-    <t>Needs review</t>
-  </si>
-  <si>
     <t>Assigned to</t>
   </si>
   <si>
@@ -101,12 +92,6 @@
     <t>DS</t>
   </si>
   <si>
-    <t>MM</t>
-  </si>
-  <si>
-    <t>Needs SI45i change</t>
-  </si>
-  <si>
     <t>Created as TC17</t>
   </si>
   <si>
@@ -114,23 +99,19 @@
   </si>
   <si>
     <t>Created as TC19</t>
+  </si>
+  <si>
+    <t>SI45i</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,14 +149,27 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -220,10 +214,9 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -236,26 +229,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -541,24 +535,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:D27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="5" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="33.75" x14ac:dyDescent="0.5">
@@ -577,20 +571,20 @@
       <c r="D6" s="12"/>
     </row>
     <row r="8" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -612,9 +606,9 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="8"/>
+      <c r="G10" s="7"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -627,7 +621,7 @@
       <c r="D11" s="2">
         <v>42.43</v>
       </c>
-      <c r="E11" s="5" t="str">
+      <c r="E11" s="16" t="str">
         <f t="shared" ref="E11:E29" si="0">"S1000 QA TC"&amp;F11</f>
         <v>S1000 QA TC16</v>
       </c>
@@ -635,14 +629,14 @@
         <f t="shared" ref="F11:F12" si="1">F12+1</f>
         <v>16</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="G11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I11" t="s">
-        <v>25</v>
+      <c r="H11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -655,7 +649,7 @@
       <c r="D12" s="2">
         <v>48.99</v>
       </c>
-      <c r="E12" s="5" t="str">
+      <c r="E12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC15</v>
       </c>
@@ -663,11 +657,11 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>20</v>
+      <c r="G12" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -680,7 +674,7 @@
       <c r="D13" s="2">
         <v>57.45</v>
       </c>
-      <c r="E13" s="5" t="str">
+      <c r="E13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC14</v>
       </c>
@@ -688,11 +682,11 @@
         <f>F14+1</f>
         <v>14</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>20</v>
+      <c r="G13" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -705,7 +699,7 @@
       <c r="D14" s="2">
         <v>64.81</v>
       </c>
-      <c r="E14" s="5" t="str">
+      <c r="E14" s="16" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC13</v>
       </c>
@@ -713,40 +707,40 @@
         <f>F19+1</f>
         <v>13</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="G14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I14" t="s">
-        <v>24</v>
+      <c r="H14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="8"/>
+      <c r="G15" s="7"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -768,9 +762,9 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="8"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -783,7 +777,7 @@
       <c r="D19" s="2">
         <v>58.09</v>
       </c>
-      <c r="E19" s="5" t="str">
+      <c r="E19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC12</v>
       </c>
@@ -791,11 +785,11 @@
         <f t="shared" ref="F19:F20" si="2">F20+1</f>
         <v>12</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>20</v>
+      <c r="G19" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -808,7 +802,7 @@
       <c r="D20" s="2">
         <v>65.38</v>
       </c>
-      <c r="E20" s="5" t="str">
+      <c r="E20" s="16" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC11</v>
       </c>
@@ -816,14 +810,14 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>23</v>
+      <c r="G20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -836,7 +830,7 @@
       <c r="D21" s="2">
         <v>75</v>
       </c>
-      <c r="E21" s="5" t="str">
+      <c r="E21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC10</v>
       </c>
@@ -844,11 +838,11 @@
         <f>F22+1</f>
         <v>10</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>20</v>
+      <c r="G21" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -861,7 +855,7 @@
       <c r="D22" s="2">
         <v>83.52</v>
       </c>
-      <c r="E22" s="5" t="str">
+      <c r="E22" s="4" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC9</v>
       </c>
@@ -869,47 +863,47 @@
         <f>F27+1</f>
         <v>9</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>20</v>
+      <c r="G22" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="5"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="8"/>
+      <c r="G23" s="7"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B24" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="B24" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
       <c r="E24" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="15" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="11"/>
@@ -918,25 +912,25 @@
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="4"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="8"/>
+      <c r="G26" s="7"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="4">
-        <v>16.97</v>
-      </c>
-      <c r="D27" s="4">
-        <v>42.43</v>
-      </c>
-      <c r="E27" s="5" t="str">
+      <c r="C27" s="15">
+        <v>25.3</v>
+      </c>
+      <c r="D27" s="15">
+        <v>63.25</v>
+      </c>
+      <c r="E27" s="4" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC8</v>
       </c>
@@ -944,24 +938,24 @@
         <f t="shared" ref="F27:F28" si="3">F28+1</f>
         <v>8</v>
       </c>
-      <c r="G27" s="8" t="s">
-        <v>21</v>
+      <c r="G27" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="4">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="D28" s="4">
-        <v>48.99</v>
-      </c>
-      <c r="E28" s="5" t="str">
+      <c r="C28" s="15">
+        <v>28.28</v>
+      </c>
+      <c r="D28" s="15">
+        <v>70.709999999999994</v>
+      </c>
+      <c r="E28" s="4" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC7</v>
       </c>
@@ -969,25 +963,25 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="G28" s="8" t="s">
-        <v>21</v>
+      <c r="G28" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="4">
-        <v>22.98</v>
-      </c>
-      <c r="D29" s="4">
-        <v>57.45</v>
-      </c>
-      <c r="E29" s="5" t="str">
+      <c r="C29" s="15">
+        <v>32.25</v>
+      </c>
+      <c r="D29" s="15">
+        <v>80.62</v>
+      </c>
+      <c r="E29" s="4" t="str">
         <f t="shared" si="0"/>
         <v>S1000 QA TC6</v>
       </c>
@@ -995,24 +989,24 @@
         <f>F30+1</f>
         <v>6</v>
       </c>
-      <c r="G29" s="8" t="s">
-        <v>21</v>
+      <c r="G29" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="4">
-        <v>25.92</v>
-      </c>
-      <c r="D30" s="4">
-        <v>64.81</v>
-      </c>
-      <c r="E30" s="5" t="str">
+      <c r="C30" s="15">
+        <v>35.78</v>
+      </c>
+      <c r="D30" s="15">
+        <v>89.44</v>
+      </c>
+      <c r="E30" s="4" t="str">
         <f>"S1000 QA TC"&amp;F30</f>
         <v>S1000 QA TC5</v>
       </c>
@@ -1020,37 +1014,37 @@
         <f>F35+1</f>
         <v>5</v>
       </c>
-      <c r="G30" s="8" t="s">
-        <v>21</v>
+      <c r="G30" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="5"/>
+      <c r="E31" s="4"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="8"/>
+      <c r="G31" s="7"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B32" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
+      <c r="B32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
       <c r="E32" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -1072,9 +1066,9 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="5"/>
+      <c r="E34" s="4"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="8"/>
+      <c r="G34" s="7"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -1087,18 +1081,18 @@
       <c r="D35" s="2">
         <v>78.58</v>
       </c>
-      <c r="E35" s="5" t="str">
+      <c r="E35" s="4" t="str">
         <f t="shared" ref="E35:E37" si="4">"S1000 QA TC"&amp;F35</f>
         <v>S1000 QA TC4</v>
       </c>
       <c r="F35" s="2">
         <v>4</v>
       </c>
-      <c r="G35" s="8" t="s">
-        <v>20</v>
+      <c r="G35" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -1111,18 +1105,18 @@
       <c r="D36" s="2">
         <v>86.46</v>
       </c>
-      <c r="E36" s="5" t="str">
+      <c r="E36" s="4" t="str">
         <f t="shared" si="4"/>
         <v>S1000 QA TC3</v>
       </c>
       <c r="F36" s="2">
         <v>3</v>
       </c>
-      <c r="G36" s="8" t="s">
-        <v>20</v>
+      <c r="G36" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -1135,18 +1129,18 @@
       <c r="D37" s="2">
         <v>97.08</v>
       </c>
-      <c r="E37" s="5" t="str">
+      <c r="E37" s="4" t="str">
         <f t="shared" si="4"/>
         <v>S1000 QA TC2</v>
       </c>
       <c r="F37" s="2">
         <v>2</v>
       </c>
-      <c r="G37" s="8" t="s">
-        <v>20</v>
+      <c r="G37" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -1159,39 +1153,39 @@
       <c r="D38" s="2">
         <v>106.65</v>
       </c>
-      <c r="E38" s="5" t="str">
+      <c r="E38" s="4" t="str">
         <f>"S1000 QA TC"&amp;F38</f>
         <v>S1000 QA TC1</v>
       </c>
       <c r="F38" s="2">
         <v>1</v>
       </c>
-      <c r="G38" s="8" t="s">
-        <v>20</v>
+      <c r="G38" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="E8:E9"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1199,6 +1193,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Notes xmlns="874d5487-6c76-4636-9554-18c8210b1644" xsi:nil="true"/>
+    <TaxCatchAll xmlns="053b13a0-8fcf-4745-a4a1-7bc77e471615" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="874d5487-6c76-4636-9554-18c8210b1644">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CE6C5D91432E0C44B4C6A820EB7148C0" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7bf22301abfb8b95bc051eca2bbc6e31">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="874d5487-6c76-4636-9554-18c8210b1644" xmlns:ns3="053b13a0-8fcf-4745-a4a1-7bc77e471615" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b6d9a428d9d7edc7a0a919696afeea0" ns2:_="" ns3:_="">
     <xsd:import namespace="874d5487-6c76-4636-9554-18c8210b1644"/>
@@ -1441,28 +1456,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Notes xmlns="874d5487-6c76-4636-9554-18c8210b1644" xsi:nil="true"/>
-    <TaxCatchAll xmlns="053b13a0-8fcf-4745-a4a1-7bc77e471615" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="874d5487-6c76-4636-9554-18c8210b1644">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4DDB590-B31D-4E3A-91E0-F94966B82335}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACAC892F-15D7-4937-AF88-9DDDD5A9DFE5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="053b13a0-8fcf-4745-a4a1-7bc77e471615"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="874d5487-6c76-4636-9554-18c8210b1644"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A22604BF-35E4-4972-8131-FFAD3720D651}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1479,23 +1498,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACAC892F-15D7-4937-AF88-9DDDD5A9DFE5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="874d5487-6c76-4636-9554-18c8210b1644"/>
-    <ds:schemaRef ds:uri="053b13a0-8fcf-4745-a4a1-7bc77e471615"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4DDB590-B31D-4E3A-91E0-F94966B82335}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>